<commit_message>
Finalizado a segunda parte do pacote que carrega as Tmp´s Denormalizadas da Tabela de Lançamentos e da Tabela de CTR_MAPEIA_CATEGORIA
</commit_message>
<xml_diff>
--- a/_Files/Categorias.xlsx
+++ b/_Files/Categorias.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repository\project\my-personal-finance\_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.2\Time Capsule\Danielle\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="225"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
@@ -378,12 +378,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -398,8 +404,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +729,12 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>90</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -729,6 +742,12 @@
       </c>
       <c r="B3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,6 +757,12 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -746,6 +771,12 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -754,13 +785,25 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -768,7 +811,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,7 +825,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -784,7 +839,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,7 +853,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,7 +867,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -808,7 +881,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,7 +895,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -824,7 +909,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,746 +923,1297 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>66</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78">
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="C84">
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="C86">
+        <v>2</v>
+      </c>
+      <c r="D86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="C87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="C93">
+        <v>2</v>
+      </c>
+      <c r="D93">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="C95">
+        <v>2</v>
+      </c>
+      <c r="D95">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C96">
+        <v>2</v>
+      </c>
+      <c r="D96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="C97">
+        <v>2</v>
+      </c>
+      <c r="D97">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>105</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>87</v>
+      </c>
+      <c r="C104">
+        <v>2</v>
+      </c>
+      <c r="D104">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>88</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>89</v>
+      </c>
+      <c r="C106">
+        <v>2</v>
+      </c>
+      <c r="D106">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107">
         <v>106</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>104</v>
-      </c>
-      <c r="B104" t="s">
+      <c r="B107" t="s">
+        <v>90</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108">
         <v>107</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>106</v>
-      </c>
-      <c r="B105" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106">
-        <v>107</v>
-      </c>
-      <c r="B106" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107">
-        <v>108</v>
-      </c>
-      <c r="B107" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108">
-        <v>109</v>
-      </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>91</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F108">
+    <sortCondition ref="B2:B108"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>